<commit_message>
fix: updated grass varialbe
</commit_message>
<xml_diff>
--- a/dictionaries/outcome/1_4/1_4_yearly_rep.xlsx
+++ b/dictionaries/outcome/1_4/1_4_yearly_rep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sidohaakma/Documents/Development/Visual/ds-dictionaries/dictionaries/outcome/1_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FBE5BD-842E-9449-88F6-066DD5D068BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7013B26-4334-4A43-B458-FEBA0C921CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="398">
   <si>
     <t>name</t>
   </si>
@@ -1220,7 +1220,7 @@
     <t>inh_all_sens_IgE_GRASS_</t>
   </si>
   <si>
-    <t>inhalant allergic sensitization to grass, measured by skin prick test</t>
+    <t>inhalant allergic senzitization to grass, measured by IgE</t>
   </si>
 </sst>
 </file>
@@ -1857,7 +1857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG139"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A117" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A135" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
@@ -3867,12 +3867,12 @@
         <v>396</v>
       </c>
       <c r="B139" s="24" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C139" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D139" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3888,10 +3888,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D261"/>
+  <dimension ref="A1:D259"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A224" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B261" sqref="B261"/>
+    <sheetView showGridLines="0" topLeftCell="A224" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A261" sqref="A260:XFD261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7527,34 +7527,6 @@
         <v>395</v>
       </c>
     </row>
-    <row r="260" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A260" s="25" t="s">
-        <v>396</v>
-      </c>
-      <c r="B260" s="17">
-        <v>0</v>
-      </c>
-      <c r="C260" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="D260" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="261" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A261" s="25" t="s">
-        <v>396</v>
-      </c>
-      <c r="B261" s="17">
-        <v>1</v>
-      </c>
-      <c r="C261" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="D261" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="2048"/>

</xml_diff>